<commit_message>
Thêm thiết kế lưu trữ Quản lý đơn hàng
</commit_message>
<xml_diff>
--- a/report/bang-yeu-cau-chuc-nang.xlsx
+++ b/report/bang-yeu-cau-chuc-nang.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12510"/>
+    <workbookView windowWidth="28800" windowHeight="12510" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Quản lý nhân viên" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,11 @@
     <sheet name="Thống kê" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:F19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
   <si>
     <t>STT</t>
   </si>
@@ -226,6 +225,9 @@
   <si>
     <t>Cho phép thêm, xóa, cập nhật 
 thông tin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Quản lý khách hàng</t>
@@ -310,8 +312,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -360,6 +362,51 @@
       <color theme="1"/>
       <name val="Oswald"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -370,11 +417,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -394,24 +463,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,28 +480,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -462,29 +494,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -497,14 +507,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -527,13 +529,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,169 +703,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,41 +753,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -804,8 +771,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -835,6 +802,41 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -853,15 +855,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -871,130 +873,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1354,7 +1356,7 @@
   <sheetPr/>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
@@ -1579,7 +1581,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="5"/>
@@ -1663,16 +1665,16 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A1" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="68.5714285714286" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="3.85714285714286" customWidth="1"/>
     <col min="2" max="2" width="3.42857142857143" customWidth="1"/>
-    <col min="3" max="3" width="18.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="43.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="68.5714285714286" customWidth="1"/>
+    <col min="3" max="3" width="5.85714285714286" customWidth="1"/>
+    <col min="4" max="4" width="10.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="22.5714285714286" customWidth="1"/>
     <col min="7" max="16384" width="68.5714285714286" customWidth="1"/>
   </cols>
@@ -1784,17 +1786,16 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A1" sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="78.5714285714286" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="15.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="12.7142857142857" customWidth="1"/>
     <col min="2" max="2" width="3.42857142857143" customWidth="1"/>
-    <col min="3" max="3" width="23.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="34.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="23.1428571428571" customWidth="1"/>
+    <col min="3" max="4" width="12.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="6.57142857142857" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="16384" width="78.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1887,24 +1888,26 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="A1" sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="93.1428571428571" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="17.1428571428571" customWidth="1"/>
+    <col min="1" max="1" width="7.28571428571429" customWidth="1"/>
     <col min="2" max="2" width="3.42857142857143" customWidth="1"/>
-    <col min="3" max="3" width="18.7142857142857" customWidth="1"/>
-    <col min="4" max="4" width="41.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="26.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="77.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="13.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="17.7142857142857" customWidth="1"/>
+    <col min="5" max="5" width="13.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="10.2857142857143" customWidth="1"/>
     <col min="7" max="31" width="93.1428571428571" customWidth="1"/>
     <col min="32" max="32" width="92.1428571428571" customWidth="1"/>
     <col min="33" max="16384" width="93.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="24" spans="1:6">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1923,19 +1926,19 @@
     </row>
     <row r="2" ht="24.75" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>10</v>
@@ -1944,19 +1947,19 @@
     <row r="3" ht="49.5" spans="1:6">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1973,8 +1976,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="62.5714285714286" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -2008,19 +2011,19 @@
     </row>
     <row r="2" ht="49.5" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>10</v>
@@ -2029,16 +2032,16 @@
     <row r="3" ht="24.75" spans="1:6">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>10</v>
@@ -2047,16 +2050,16 @@
     <row r="4" ht="49.5" spans="1:6">
       <c r="A4" s="3"/>
       <c r="B4" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>10</v>
@@ -2065,16 +2068,16 @@
     <row r="5" ht="49.5" spans="1:6">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>10</v>

</xml_diff>